<commit_message>
add weapons + inventory + enemy + player stats + CaracterPanel + Update timesheet
</commit_message>
<xml_diff>
--- a/TimeSpend.xlsx
+++ b/TimeSpend.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arne\Desktop\NitroGamesSecretOfEvermore\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arne\Desktop\PROJECTS\SecretOfEvermore\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>19:00-19:30</t>
   </si>
@@ -42,6 +42,90 @@
   </si>
   <si>
     <t>setup player systems + gamemanager + create repository</t>
+  </si>
+  <si>
+    <t>13:35-14:07</t>
+  </si>
+  <si>
+    <t>14:33-15:00</t>
+  </si>
+  <si>
+    <t>14:15-14:32</t>
+  </si>
+  <si>
+    <t>16:20-17:35</t>
+  </si>
+  <si>
+    <t>19:30-21:15</t>
+  </si>
+  <si>
+    <t>21:30-22:30</t>
+  </si>
+  <si>
+    <t>movement navmesh</t>
+  </si>
+  <si>
+    <t>camera</t>
+  </si>
+  <si>
+    <t>player switching</t>
+  </si>
+  <si>
+    <t>HUD</t>
+  </si>
+  <si>
+    <t>stats</t>
+  </si>
+  <si>
+    <t>camera + player switching</t>
+  </si>
+  <si>
+    <t>13:30-13:40</t>
+  </si>
+  <si>
+    <t>13:40-15:44</t>
+  </si>
+  <si>
+    <t>15:50-16:22</t>
+  </si>
+  <si>
+    <t>17:20-18:00</t>
+  </si>
+  <si>
+    <t>19:34-19:54</t>
+  </si>
+  <si>
+    <t>weapons</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>enemy</t>
+  </si>
+  <si>
+    <t>enemy attack + damage system on the player</t>
+  </si>
+  <si>
+    <t>20:00-20:38</t>
+  </si>
+  <si>
+    <t>weapon switching + player stats + inventory</t>
+  </si>
+  <si>
+    <t>21:30-00:30</t>
+  </si>
+  <si>
+    <t>total time</t>
+  </si>
+  <si>
+    <t>time worked</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>2,5</t>
   </si>
 </sst>
 </file>
@@ -83,7 +167,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -99,7 +183,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -395,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L9"/>
+  <dimension ref="B3:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +490,9 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="54.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -413,10 +500,16 @@
         <v>43088</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -430,6 +523,15 @@
       <c r="C4" t="s">
         <v>1</v>
       </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -438,11 +540,23 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
+      <c r="D5">
+        <v>120</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>43089</v>
       </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -450,6 +564,207 @@
       </c>
       <c r="C9" t="s">
         <v>5</v>
+      </c>
+      <c r="D9">
+        <v>120</v>
+      </c>
+      <c r="F9">
+        <v>120</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>43095</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>32</v>
+      </c>
+      <c r="F12">
+        <f>D12+D13+D14+D15+D16+D17</f>
+        <v>316</v>
+      </c>
+      <c r="G12">
+        <f>F12/60</f>
+        <v>5.2666666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>43096</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <f>D20+D21+D22+D24+D23+D25+D26</f>
+        <v>444</v>
+      </c>
+      <c r="G20">
+        <f>F20/60</f>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>43097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>